<commit_message>
updating the or-tools implementation
</commit_message>
<xml_diff>
--- a/ta-scheduler-ortools/data/availability_Template.xlsx
+++ b/ta-scheduler-ortools/data/availability_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danialnoorizadeh/Code/ShiftScheduler/OR-tools/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danialnoorizadeh/Code/ShiftScheduler/ta-scheduler-ortools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE0A7E9-848B-7641-AC17-5A63CACEF08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558A1CBC-0990-FD43-AAA9-75BF6ED92A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="500" windowWidth="21800" windowHeight="13920" xr2:uid="{98118C80-EDF3-C141-9DFA-EEAB9BD2538B}"/>
   </bookViews>
@@ -1170,7 +1170,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>